<commit_message>
Prepared for upload of steel cycle in-use stocks by 4 product groups.
</commit_message>
<xml_diff>
--- a/IEDC_Classification_fill/general_product_categories_data.xlsx
+++ b/IEDC_Classification_fill/general_product_categories_data.xlsx
@@ -130,16 +130,16 @@
     <t>reserved</t>
   </si>
   <si>
-    <t>buildings, construction, and infrastructure</t>
-  </si>
-  <si>
-    <t>machinery</t>
-  </si>
-  <si>
     <t>vehicles and other transport equipment</t>
   </si>
   <si>
-    <t>appliances, packaging, and other</t>
+    <t>industrial machinery</t>
+  </si>
+  <si>
+    <t>buildings - construction - infrastructure</t>
+  </si>
+  <si>
+    <t>appliances - packaging - other</t>
   </si>
 </sst>
 </file>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,7 +846,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -862,7 +862,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>